<commit_message>
script merge comunidades iccaa y media com
</commit_message>
<xml_diff>
--- a/informes/informe_madrid.xlsx
+++ b/informes/informe_madrid.xlsx
@@ -401,7 +401,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1.529</v>
+        <v>1.519</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -441,7 +441,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>1.689</v>
+        <v>1.679</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -481,16 +481,16 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>1.715</v>
+        <v>1.709</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CEPSA</t>
+          <t>REPSOL</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CARRETERA M-405 KM. 6</t>
+          <t>CL MADRID, 52</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CTRA. M-505 km 5,5</t>
+          <t>CALLE COPENHAGUES/N, S/N</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CARRETERA M-505 km 5.5</t>
+          <t>A-6 km 25,5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -550,7 +550,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>A-6 km 25,5</t>
+          <t>CTRA. M-505 km 5,5</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CALLE COPENHAGUES/N, S/N</t>
+          <t>CARRETERA M-505 km 5.5</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -581,16 +581,16 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>1.729</v>
+        <v>1.719</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>REPSOL HUMANES</t>
+          <t>BP VALDONAIRE</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>AVENIDA LA INDUSTRIA, S/N</t>
+          <t>CARRETERA AVD.DE LA INDUSTRIA KM. 15</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -601,16 +601,16 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>1.729</v>
+        <v>1.719</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BP VALDONAIRE</t>
+          <t>BP HUMANES - EL MOLINO</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CARRETERA AVD.DE LA INDUSTRIA KM. 15</t>
+          <t>AVENIDA DE LAS FLORES, 2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -621,16 +621,16 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>1.729</v>
+        <v>1.719</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BP HUMANES - EL MOLINO</t>
+          <t>CEPSA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>AVENIDA DE LAS FLORES, 2</t>
+          <t>CARRETERA M-405 KM. 5,6</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -641,16 +641,16 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>1.729</v>
+        <v>1.719</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>REPSOL</t>
+          <t>REPSOL HUMANES</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CL MADRID, 52</t>
+          <t>AVENIDA LA INDUSTRIA, S/N</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -661,36 +661,36 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>1.729</v>
+        <v>1.719</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BP LAS ROZAS</t>
+          <t>REPSOL</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CL LAS CRUCES  S/N</t>
+          <t>CARRETERA AVENIDA  DE LA INDUSTRIA , 46 KM. 1,1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ROZAS DE MADRID (LAS)</t>
+          <t>HUMANES DE MADRID</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>1.729</v>
+        <v>1.719</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>REPSOL</t>
+          <t>BP LAS ROZAS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CR A-6, 20,3</t>
+          <t>CL LAS CRUCES  S/N</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -701,36 +701,36 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>1.735</v>
+        <v>1.719</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CEPSA</t>
+          <t>REPSOL</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CARRETERA M-405 KM. 5,6</t>
+          <t>CR A-6, 20,3</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>HUMANES DE MADRID</t>
+          <t>ROZAS DE MADRID (LAS)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>1.739</v>
+        <v>1.725</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>REPSOL</t>
+          <t>CEPSA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CARRETERA AVENIDA  DE LA INDUSTRIA , 46 KM. 1,1</t>
+          <t>CARRETERA M-405 KM. 6</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">

</xml_diff>

<commit_message>
poblacion total,m y f por municipio
</commit_message>
<xml_diff>
--- a/informes/informe_madrid.xlsx
+++ b/informes/informe_madrid.xlsx
@@ -381,7 +381,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1.509</v>
+        <v>1.497</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -401,7 +401,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>1.519</v>
+        <v>1.514</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -421,7 +421,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>1.639</v>
+        <v>1.599</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -441,16 +441,16 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>1.679</v>
+        <v>1.649</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>GALP</t>
+          <t>CARREFOUR</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CTRA. N-VI km 21,700</t>
+          <t>CARRETERA MADRID-LA CORUÑA KM. 22</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -461,16 +461,16 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>1.699</v>
+        <v>1.669</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CARREFOUR</t>
+          <t>GALP</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CARRETERA MADRID-LA CORUÑA KM. 22</t>
+          <t>CTRA. N-VI km 21,700</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -481,7 +481,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>1.709</v>
+        <v>1.688</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -490,18 +490,18 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CL MADRID, 52</t>
+          <t>CALLE COPENHAGUES/N, S/N</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>HUMANES DE MADRID</t>
+          <t>ROZAS DE MADRID (LAS)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>1.718</v>
+        <v>1.688</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -510,7 +510,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CALLE COPENHAGUES/N, S/N</t>
+          <t>A-6 km 25,5</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -521,7 +521,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>1.718</v>
+        <v>1.688</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -530,7 +530,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>A-6 km 25,5</t>
+          <t>CTRA. M-505 km 5,5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -541,7 +541,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>1.718</v>
+        <v>1.688</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CTRA. M-505 km 5,5</t>
+          <t>CARRETERA M-505 km 5.5</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -561,36 +561,36 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>1.718</v>
+        <v>1.689</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>REPSOL</t>
+          <t>CEPSA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CARRETERA M-505 km 5.5</t>
+          <t>CARRETERA M-405 KM. 6</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ROZAS DE MADRID (LAS)</t>
+          <t>HUMANES DE MADRID</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>1.719</v>
+        <v>1.699</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BP VALDONAIRE</t>
+          <t>REPSOL HUMANES</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CARRETERA AVD.DE LA INDUSTRIA KM. 15</t>
+          <t>AVENIDA LA INDUSTRIA, S/N</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -601,16 +601,16 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>1.719</v>
+        <v>1.699</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BP HUMANES - EL MOLINO</t>
+          <t>CEPSA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AVENIDA DE LAS FLORES, 2</t>
+          <t>CARRETERA M-405 KM. 5,6</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -621,16 +621,16 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>1.719</v>
+        <v>1.699</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CEPSA</t>
+          <t>REPSOL</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CARRETERA M-405 KM. 5,6</t>
+          <t>CL MADRID, 52</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -641,16 +641,16 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>1.719</v>
+        <v>1.709</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>REPSOL HUMANES</t>
+          <t>BP VALDONAIRE</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>AVENIDA LA INDUSTRIA, S/N</t>
+          <t>CARRETERA AVD.DE LA INDUSTRIA KM. 15</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -661,16 +661,16 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>1.719</v>
+        <v>1.709</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>REPSOL</t>
+          <t>BP HUMANES - EL MOLINO</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>CARRETERA AVENIDA  DE LA INDUSTRIA , 46 KM. 1,1</t>
+          <t>AVENIDA DE LAS FLORES, 2</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -681,27 +681,27 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>1.719</v>
+        <v>1.709</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BP LAS ROZAS</t>
+          <t>REPSOL</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CL LAS CRUCES  S/N</t>
+          <t>CARRETERA AVENIDA  DE LA INDUSTRIA , 46 KM. 1,1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>ROZAS DE MADRID (LAS)</t>
+          <t>HUMANES DE MADRID</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>1.719</v>
+        <v>1.709</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -721,27 +721,27 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>1.725</v>
+        <v>1.709</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CEPSA</t>
+          <t>BP LAS ROZAS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CARRETERA M-405 KM. 6</t>
+          <t>CL LAS CRUCES  S/N</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>HUMANES DE MADRID</t>
+          <t>ROZAS DE MADRID (LAS)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>1.924</v>
+        <v>1.861</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>

</xml_diff>